<commit_message>
Test 5 er i gang
</commit_message>
<xml_diff>
--- a/IntegrationstestPlan.xlsx
+++ b/IntegrationstestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au588570_uni_au_dk/Documents/4. semester/Software T/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troel\OneDrive - Aarhus universitet\Skole\Uni\4. semester\SWT\MicrowaveOvenGrp9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB9309A1-191A-4032-B9BC-5D55C5A05796}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7C6FCA-E8F0-4196-BD2F-87AEA6B54D56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{1352ABC7-6360-4182-BFD5-E3A943094EFF}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" xr2:uid="{1352ABC7-6360-4182-BFD5-E3A943094EFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="14">
   <si>
     <t>Step #</t>
   </si>
@@ -79,10 +79,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,9 +115,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,24 +437,24 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -500,7 +509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -523,7 +532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -552,7 +561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -578,33 +587,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -624,7 +637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -644,7 +657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -673,7 +686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -684,7 +697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -713,7 +726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -747,5 +760,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>